<commit_message>
Update documentation for RunCommands changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="456">
   <si>
     <t>Add</t>
   </si>
@@ -1726,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3129,6 +3129,12 @@
       <c r="B144" t="s">
         <v>371</v>
       </c>
+      <c r="C144" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
@@ -3909,11 +3915,11 @@
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C227" s="3">
         <f>COUNTIF(C2:C226,"=Y")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D227" s="3">
         <f>COUNTIF(D2:D226,"=Y")</f>
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove MexicoCSMN input type - obsolete.  Update documentation to version 11.06.00 for release.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="458">
   <si>
     <t>Add</t>
   </si>
@@ -1392,6 +1392,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>ReadExcelWorkbook</t>
+  </si>
+  <si>
+    <t>Read an Excel workbook into memory so that it can be manipulated.</t>
   </si>
 </sst>
 </file>
@@ -1724,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D227"/>
+  <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1895,6 +1901,12 @@
       <c r="B13" t="s">
         <v>236</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2790,192 +2802,192 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>456</v>
       </c>
       <c r="B106" t="s">
-        <v>333</v>
+        <v>457</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>354</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>454</v>
+        <v>353</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>454</v>
@@ -2986,126 +2998,126 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>358</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>454</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
-        <v>368</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>454</v>
+        <v>367</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>454</v>
@@ -3116,100 +3128,100 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" t="s">
-        <v>371</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>454</v>
+        <v>370</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145" t="s">
-        <v>372</v>
+        <v>371</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B146" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B147" t="s">
-        <v>374</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>454</v>
+        <v>373</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151" t="s">
-        <v>378</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D151" s="3" t="s">
-        <v>454</v>
+        <v>377</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>454</v>
@@ -3220,180 +3232,180 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B153" t="s">
-        <v>380</v>
+        <v>379</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>382</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156" t="s">
-        <v>383</v>
+        <v>382</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B157" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B158" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B159" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B160" t="s">
-        <v>387</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>454</v>
+        <v>386</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B161" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B162" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B163" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B164" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B165" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B166" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B167" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B169" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B170" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B171" t="s">
-        <v>398</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>454</v>
+        <v>397</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B172" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>454</v>
@@ -3404,10 +3416,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B173" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>454</v>
@@ -3418,56 +3430,56 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B174" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B175" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B176" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B177" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B178" t="s">
-        <v>405</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B179" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>454</v>
@@ -3478,186 +3490,186 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B180" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B181" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B182" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B183" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B185" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B186" t="s">
-        <v>413</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>454</v>
+        <v>412</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B187" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B188" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B189" t="s">
-        <v>418</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>454</v>
+        <v>415</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B190" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B191" t="s">
-        <v>417</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>454</v>
+        <v>416</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B192" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B193" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B194" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B195" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B196" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B197" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B198" t="s">
-        <v>425</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B199" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>454</v>
@@ -3668,136 +3680,136 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B200" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B201" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B202" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B203" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B204" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B205" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B206" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B207" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B208" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214" t="s">
-        <v>441</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D214" s="3" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C215" s="3" t="s">
         <v>454</v>
@@ -3808,10 +3820,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>454</v>
@@ -3822,64 +3834,64 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217" t="s">
-        <v>444</v>
+        <v>443</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B222" t="s">
-        <v>449</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B223" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>454</v>
@@ -3890,36 +3902,50 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B224" t="s">
-        <v>452</v>
+        <v>450</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B225" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>223</v>
+      </c>
+      <c r="B226" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
         <v>224</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B227" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C227" s="3">
-        <f>COUNTIF(C2:C226,"=Y")</f>
-        <v>56</v>
-      </c>
-      <c r="D227" s="3">
-        <f>COUNTIF(D2:D226,"=Y")</f>
-        <v>57</v>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C228" s="3">
+        <f>COUNTIF(C2:C227,"=Y")</f>
+        <v>58</v>
+      </c>
+      <c r="D228" s="3">
+        <f>COUNTIF(D2:D227,"=Y")</f>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update inventory for recent changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="458">
   <si>
     <t>Add</t>
   </si>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3885,6 +3885,12 @@
       <c r="B222" t="s">
         <v>448</v>
       </c>
+      <c r="C222" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
@@ -3941,11 +3947,11 @@
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C228" s="3">
         <f>COUNTIF(C2:C227,"=Y")</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D228" s="3">
         <f>COUNTIF(D2:D227,"=Y")</f>
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documentation for recent changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="458">
   <si>
     <t>Add</t>
   </si>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3571,6 +3571,12 @@
       <c r="B188" t="s">
         <v>414</v>
       </c>
+      <c r="C188" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
@@ -3947,11 +3953,11 @@
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C228" s="3">
         <f>COUNTIF(C2:C227,"=Y")</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D228" s="3">
         <f>COUNTIF(D2:D227,"=Y")</f>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update release notes for 11.07.03beta release.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="462">
   <si>
     <t>Add</t>
   </si>
@@ -1398,6 +1398,18 @@
   </si>
   <si>
     <t>Read an Excel workbook into memory so that it can be manipulated.</t>
+  </si>
+  <si>
+    <t>WriteTimeSeriesToHydroJSON</t>
+  </si>
+  <si>
+    <t>Write time series to HydroJSON text file, used with Reclamation Pisces.</t>
+  </si>
+  <si>
+    <t>ReadReclamationPisces</t>
+  </si>
+  <si>
+    <t>Read time series and ensembles from the US Bureau of Reclamation Pisces database.</t>
   </si>
 </sst>
 </file>
@@ -1730,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D228"/>
+  <dimension ref="A1:D230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2912,96 +2924,96 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>460</v>
       </c>
       <c r="B119" t="s">
-        <v>345</v>
+        <v>461</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B120" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B121" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B122" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B123" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B124" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B127" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B128" t="s">
-        <v>354</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>454</v>
+        <v>353</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>454</v>
@@ -3012,126 +3024,126 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B130" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B131" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B132" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>358</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>454</v>
+        <v>359</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B137" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B138" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B139" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B140" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B141" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>368</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>454</v>
+        <v>367</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B143" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>454</v>
@@ -3142,100 +3154,100 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B144" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B145" t="s">
-        <v>371</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>454</v>
+        <v>370</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B146" t="s">
-        <v>372</v>
+        <v>371</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B147" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B148" t="s">
-        <v>374</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>454</v>
+        <v>373</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B149" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B150" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B151" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B152" t="s">
-        <v>378</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D152" s="3" t="s">
-        <v>454</v>
+        <v>377</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B153" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>454</v>
@@ -3246,180 +3258,180 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B154" t="s">
-        <v>380</v>
+        <v>379</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B155" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B156" t="s">
-        <v>382</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D156" s="3" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B157" t="s">
-        <v>383</v>
+        <v>382</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B158" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B159" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B160" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B161" t="s">
-        <v>387</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>454</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B162" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B163" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B164" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B165" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B166" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B167" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B168" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B169" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B170" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B171" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B172" t="s">
-        <v>398</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>454</v>
+        <v>397</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B173" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>454</v>
@@ -3430,10 +3442,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B174" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>454</v>
@@ -3444,56 +3456,56 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B175" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B176" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B177" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B178" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B179" t="s">
-        <v>405</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B180" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>454</v>
@@ -3504,72 +3516,72 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B181" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B182" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B183" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B184" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B185" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B186" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B187" t="s">
-        <v>413</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D187" s="3" t="s">
-        <v>454</v>
+        <v>412</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B188" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>454</v>
@@ -3580,116 +3592,116 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B189" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B190" t="s">
-        <v>418</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>454</v>
+        <v>415</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B191" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B192" t="s">
-        <v>417</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>454</v>
+        <v>416</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B193" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B194" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B195" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B196" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B197" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B198" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B199" t="s">
-        <v>425</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B200" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>454</v>
@@ -3700,136 +3712,136 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B201" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B202" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B203" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B204" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B205" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B206" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B208" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B209" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B210" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B211" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B212" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B213" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B214" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B215" t="s">
-        <v>441</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D215" s="3" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B216" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C216" s="3" t="s">
         <v>454</v>
@@ -3840,10 +3852,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B217" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>454</v>
@@ -3854,56 +3866,56 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B218" t="s">
-        <v>444</v>
+        <v>443</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B219" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B220" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B221" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B222" t="s">
-        <v>448</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B223" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>454</v>
@@ -3914,10 +3926,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B224" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>454</v>
@@ -3928,36 +3940,70 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B225" t="s">
-        <v>452</v>
+        <v>450</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>223</v>
+        <v>458</v>
       </c>
       <c r="B226" t="s">
-        <v>451</v>
+        <v>459</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>222</v>
+      </c>
+      <c r="B227" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>223</v>
+      </c>
+      <c r="B228" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
         <v>224</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B229" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C228" s="3">
-        <f>COUNTIF(C2:C227,"=Y")</f>
-        <v>60</v>
-      </c>
-      <c r="D228" s="3">
-        <f>COUNTIF(D2:D227,"=Y")</f>
-        <v>61</v>
+      <c r="C229" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C230" s="3">
+        <f>COUNTIF(C2:C229,"=Y")</f>
+        <v>63</v>
+      </c>
+      <c r="D230" s="3">
+        <f>COUNTIF(D2:D229,"=Y")</f>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update release notes for release.  Update WriteTimeSeriesToDataStream documenation for recent changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="464">
   <si>
     <t>Add</t>
   </si>
@@ -1751,10 +1751,10 @@
   <dimension ref="A1:D231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C188" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
+      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2809,6 +2809,12 @@
       <c r="B104" t="s">
         <v>331</v>
       </c>
+      <c r="C104" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
@@ -3690,6 +3696,9 @@
       <c r="C195" s="3" t="s">
         <v>454</v>
       </c>
+      <c r="D195" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
@@ -4034,11 +4043,11 @@
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C231" s="3">
         <f>COUNTIF(C2:C230,"=Y")</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D231" s="3">
         <f>COUNTIF(D2:D230,"=Y")</f>
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ReadTableFromJSON command and update documentation for 11.07.05 release.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="466">
   <si>
     <t>Add</t>
   </si>
@@ -1416,6 +1416,12 @@
   </si>
   <si>
     <t>Unzip a zip file's contents</t>
+  </si>
+  <si>
+    <t>ReadTableFromJSON</t>
+  </si>
+  <si>
+    <t>Read a table from a JSON file</t>
   </si>
 </sst>
 </file>
@@ -1748,13 +1754,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D231"/>
+  <dimension ref="A1:D232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C188" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D196" sqref="D196"/>
+      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3070,124 +3076,124 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>128</v>
+        <v>464</v>
       </c>
       <c r="B132" t="s">
-        <v>357</v>
+        <v>465</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>360</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>454</v>
+        <v>357</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B134" t="s">
-        <v>359</v>
+        <v>360</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>358</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>454</v>
+        <v>359</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B139" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B140" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B141" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B142" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B143" t="s">
-        <v>368</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D143" s="3" t="s">
-        <v>454</v>
+        <v>367</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>454</v>
@@ -3198,100 +3204,100 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B145" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B146" t="s">
-        <v>371</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>454</v>
+        <v>370</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B147" t="s">
-        <v>372</v>
+        <v>371</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B148" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B149" t="s">
-        <v>374</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>454</v>
+        <v>373</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B150" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B151" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B152" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B153" t="s">
-        <v>378</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>454</v>
+        <v>377</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B154" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>454</v>
@@ -3302,180 +3308,180 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B155" t="s">
-        <v>380</v>
+        <v>379</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B156" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>382</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B158" t="s">
-        <v>383</v>
+        <v>382</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B161" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B162" t="s">
-        <v>387</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>454</v>
+        <v>386</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B163" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B164" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B165" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B166" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B167" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B168" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B169" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B170" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B171" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B172" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B173" t="s">
-        <v>398</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D173" s="3" t="s">
-        <v>454</v>
+        <v>397</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B174" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>454</v>
@@ -3486,10 +3492,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B175" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>454</v>
@@ -3500,56 +3506,56 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B176" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B177" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B178" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B179" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B180" t="s">
-        <v>405</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B181" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>454</v>
@@ -3560,72 +3566,72 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B182" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B183" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B184" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B185" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B186" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B187" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B188" t="s">
-        <v>413</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>454</v>
+        <v>412</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B189" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>454</v>
@@ -3636,130 +3642,130 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B190" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B191" t="s">
-        <v>418</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>454</v>
+        <v>415</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B192" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B193" t="s">
-        <v>417</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>454</v>
+        <v>416</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B194" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>462</v>
+        <v>190</v>
       </c>
       <c r="B195" t="s">
-        <v>463</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>454</v>
+        <v>419</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>191</v>
+        <v>462</v>
       </c>
       <c r="B196" t="s">
-        <v>420</v>
+        <v>463</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B197" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B198" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B199" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B200" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B201" t="s">
-        <v>425</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B202" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>454</v>
@@ -3770,136 +3776,136 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B203" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B204" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B205" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B206" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B207" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B208" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B209" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B210" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B211" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B212" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B213" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B214" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B215" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B216" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B217" t="s">
-        <v>441</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D217" s="3" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B218" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>454</v>
@@ -3910,10 +3916,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B219" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C219" s="3" t="s">
         <v>454</v>
@@ -3924,56 +3930,56 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B220" t="s">
-        <v>444</v>
+        <v>443</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B221" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B222" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B223" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B224" t="s">
-        <v>448</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D224" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B225" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>454</v>
@@ -3984,10 +3990,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B226" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>454</v>
@@ -3998,10 +4004,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>458</v>
+        <v>221</v>
       </c>
       <c r="B227" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>454</v>
@@ -4012,42 +4018,56 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>222</v>
+        <v>458</v>
       </c>
       <c r="B228" t="s">
-        <v>452</v>
+        <v>459</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B229" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>223</v>
+      </c>
+      <c r="B230" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
         <v>224</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>453</v>
       </c>
-      <c r="C230" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D230" s="3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C231" s="3">
-        <f>COUNTIF(C2:C230,"=Y")</f>
-        <v>68</v>
-      </c>
-      <c r="D231" s="3">
-        <f>COUNTIF(D2:D230,"=Y")</f>
-        <v>68</v>
+      <c r="C231" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C232" s="3">
+        <f>COUNTIF(C2:C231,"=Y")</f>
+        <v>69</v>
+      </c>
+      <c r="D232" s="3">
+        <f>COUNTIF(D2:D231,"=Y")</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documentation for new features.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="468">
   <si>
     <t>Add</t>
   </si>
@@ -1358,9 +1358,6 @@
     <t>Write a table to an HTML file.</t>
   </si>
   <si>
-    <t>Write a table to Excel, formatting spatial data columns into KML.</t>
-  </si>
-  <si>
     <t>Write time series properties to a file, useful for automated tests.</t>
   </si>
   <si>
@@ -1422,6 +1419,15 @@
   </si>
   <si>
     <t>Read a table from a JSON file</t>
+  </si>
+  <si>
+    <t>WriteTableToShapefile</t>
+  </si>
+  <si>
+    <t>Write a table to KML file, formatting spatial data columns into KML.</t>
+  </si>
+  <si>
+    <t>Write a table to Esri shapefile.</t>
   </si>
 </sst>
 </file>
@@ -1754,13 +1760,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D232"/>
+  <dimension ref="A1:D233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
+      <selection pane="bottomRight" activeCell="D223" sqref="D223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,10 +1799,10 @@
         <v>227</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1807,10 +1813,10 @@
         <v>228</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1821,10 +1827,10 @@
         <v>249</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1843,10 +1849,10 @@
         <v>230</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1857,10 +1863,10 @@
         <v>231</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1871,10 +1877,10 @@
         <v>232</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1901,10 +1907,10 @@
         <v>234</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1915,10 +1921,10 @@
         <v>235</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1929,10 +1935,10 @@
         <v>236</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1943,10 +1949,10 @@
         <v>237</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1973,10 +1979,10 @@
         <v>240</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1987,10 +1993,10 @@
         <v>241</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2001,10 +2007,10 @@
         <v>243</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2015,10 +2021,10 @@
         <v>242</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2069,10 +2075,10 @@
         <v>251</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2099,7 +2105,7 @@
         <v>254</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,10 +2116,10 @@
         <v>255</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,10 +2130,10 @@
         <v>256</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2258,10 +2264,10 @@
         <v>272</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2272,10 +2278,10 @@
         <v>273</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2294,10 +2300,10 @@
         <v>274</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2308,10 +2314,10 @@
         <v>281</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2330,10 +2336,10 @@
         <v>279</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2384,10 +2390,10 @@
         <v>284</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2414,10 +2420,10 @@
         <v>287</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2444,10 +2450,10 @@
         <v>290</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2458,10 +2464,10 @@
         <v>291</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2504,7 +2510,7 @@
         <v>296</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2587,7 +2593,7 @@
         <v>308</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2622,10 +2628,10 @@
         <v>312</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2644,10 +2650,10 @@
         <v>314</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2658,10 +2664,10 @@
         <v>315</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2704,10 +2710,10 @@
         <v>320</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2718,10 +2724,10 @@
         <v>321</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2732,10 +2738,10 @@
         <v>322</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2745,6 +2751,12 @@
       <c r="B96" t="s">
         <v>323</v>
       </c>
+      <c r="C96" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
@@ -2794,10 +2806,10 @@
         <v>329</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2816,10 +2828,10 @@
         <v>331</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2830,24 +2842,24 @@
         <v>332</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>455</v>
+      </c>
+      <c r="B106" t="s">
         <v>456</v>
       </c>
-      <c r="B106" t="s">
-        <v>457</v>
-      </c>
       <c r="C106" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2948,16 +2960,16 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>459</v>
+      </c>
+      <c r="B119" t="s">
         <v>460</v>
       </c>
-      <c r="B119" t="s">
-        <v>461</v>
-      </c>
       <c r="C119" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -3024,10 +3036,10 @@
         <v>352</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -3046,10 +3058,10 @@
         <v>354</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -3060,10 +3072,10 @@
         <v>355</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -3076,16 +3088,16 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>463</v>
+      </c>
+      <c r="B132" t="s">
         <v>464</v>
       </c>
-      <c r="B132" t="s">
-        <v>465</v>
-      </c>
       <c r="C132" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -3104,10 +3116,10 @@
         <v>360</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -3126,10 +3138,10 @@
         <v>358</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -3196,10 +3208,10 @@
         <v>368</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -3210,10 +3222,10 @@
         <v>369</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3232,10 +3244,10 @@
         <v>371</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3262,10 +3274,10 @@
         <v>374</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3300,10 +3312,10 @@
         <v>378</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3314,10 +3326,10 @@
         <v>379</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3344,10 +3356,10 @@
         <v>382</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3390,10 +3402,10 @@
         <v>387</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3484,10 +3496,10 @@
         <v>398</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -3498,10 +3510,10 @@
         <v>400</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -3512,10 +3524,10 @@
         <v>399</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -3558,10 +3570,10 @@
         <v>405</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3572,10 +3584,10 @@
         <v>406</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3634,10 +3646,10 @@
         <v>413</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -3648,10 +3660,10 @@
         <v>414</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -3670,10 +3682,10 @@
         <v>418</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
@@ -3692,10 +3704,10 @@
         <v>417</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
@@ -3708,16 +3720,16 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
+        <v>461</v>
+      </c>
+      <c r="B196" t="s">
         <v>462</v>
       </c>
-      <c r="B196" t="s">
-        <v>463</v>
-      </c>
       <c r="C196" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
@@ -3768,10 +3780,10 @@
         <v>425</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -3782,10 +3794,10 @@
         <v>426</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
@@ -3908,10 +3920,10 @@
         <v>441</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
@@ -3922,10 +3934,10 @@
         <v>442</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
@@ -3936,10 +3948,10 @@
         <v>443</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
@@ -3947,100 +3959,106 @@
         <v>215</v>
       </c>
       <c r="B221" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>216</v>
+        <v>465</v>
       </c>
       <c r="B222" t="s">
-        <v>445</v>
+        <v>467</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B223" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B224" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B225" t="s">
-        <v>448</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B226" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B227" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>458</v>
+        <v>221</v>
       </c>
       <c r="B228" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>222</v>
+        <v>457</v>
       </c>
       <c r="B229" t="s">
-        <v>452</v>
+        <v>458</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B230" t="s">
         <v>451</v>
@@ -4048,26 +4066,34 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>223</v>
+      </c>
+      <c r="B231" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
         <v>224</v>
       </c>
-      <c r="B231" t="s">
-        <v>453</v>
-      </c>
-      <c r="C231" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D231" s="3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C232" s="3">
-        <f>COUNTIF(C2:C231,"=Y")</f>
-        <v>69</v>
-      </c>
-      <c r="D232" s="3">
-        <f>COUNTIF(D2:D231,"=Y")</f>
-        <v>69</v>
+      <c r="B232" t="s">
+        <v>452</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C233" s="3">
+        <f>COUNTIF(C2:C232,"=Y")</f>
+        <v>71</v>
+      </c>
+      <c r="D233" s="3">
+        <f>COUNTIF(D2:D232,"=Y")</f>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add documentation for WriteTableToGeoJSON command.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="470">
   <si>
     <t>Add</t>
   </si>
@@ -1428,6 +1428,12 @@
   </si>
   <si>
     <t>Write a table to Esri shapefile.</t>
+  </si>
+  <si>
+    <t>WriteTableToGeoJSON</t>
+  </si>
+  <si>
+    <t>Write a table to GeoJSON file.</t>
   </si>
 </sst>
 </file>
@@ -1760,13 +1766,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B216" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D223" sqref="D223"/>
+      <selection pane="bottomRight" activeCell="E222" sqref="E222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2987,6 +2993,12 @@
       <c r="B121" t="s">
         <v>346</v>
       </c>
+      <c r="C121" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
@@ -3863,6 +3875,12 @@
       <c r="B211" t="s">
         <v>434</v>
       </c>
+      <c r="C211" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
@@ -3942,10 +3960,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>214</v>
+        <v>468</v>
       </c>
       <c r="B220" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>453</v>
@@ -3956,70 +3974,70 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B221" t="s">
-        <v>466</v>
+        <v>443</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>465</v>
+        <v>215</v>
       </c>
       <c r="B222" t="s">
-        <v>467</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>216</v>
+        <v>465</v>
       </c>
       <c r="B223" t="s">
-        <v>444</v>
+        <v>467</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B224" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B225" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B226" t="s">
-        <v>447</v>
-      </c>
-      <c r="C226" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D226" s="3" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B227" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>453</v>
@@ -4030,10 +4048,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B228" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C228" s="3" t="s">
         <v>453</v>
@@ -4044,10 +4062,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>457</v>
+        <v>221</v>
       </c>
       <c r="B229" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>453</v>
@@ -4058,42 +4076,56 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>222</v>
+        <v>457</v>
       </c>
       <c r="B230" t="s">
-        <v>451</v>
+        <v>458</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B231" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>223</v>
+      </c>
+      <c r="B232" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>224</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>452</v>
       </c>
-      <c r="C232" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C233" s="3">
-        <f>COUNTIF(C2:C232,"=Y")</f>
-        <v>71</v>
-      </c>
-      <c r="D233" s="3">
-        <f>COUNTIF(D2:D232,"=Y")</f>
-        <v>71</v>
+      <c r="C233" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C234" s="3">
+        <f>COUNTIF(C2:C233,"=Y")</f>
+        <v>74</v>
+      </c>
+      <c r="D234" s="3">
+        <f>COUNTIF(D2:D233,"=Y")</f>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documenation for recent changes, in particular adding GZIP support to some commands, adding ReadDelftFewsPiXml.  Also correct GenericDatabaseDataStore documentation.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="474">
   <si>
     <t>Add</t>
   </si>
@@ -1434,6 +1434,18 @@
   </si>
   <si>
     <t>Write a table to GeoJSON file.</t>
+  </si>
+  <si>
+    <t>WriteDelftFewsPiXml</t>
+  </si>
+  <si>
+    <t>Write time series to DELFT FEWS PI XML file.</t>
+  </si>
+  <si>
+    <t>ReadDelftFewsPiXml</t>
+  </si>
+  <si>
+    <t>Read time series from DELFT FEWS PI XML file.</t>
   </si>
 </sst>
 </file>
@@ -1766,13 +1778,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:D236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B216" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E222" sqref="E222"/>
+      <selection pane="bottomRight" activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3064,10 +3076,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>472</v>
       </c>
       <c r="B129" t="s">
-        <v>354</v>
+        <v>473</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>453</v>
@@ -3078,10 +3090,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>453</v>
@@ -3092,146 +3104,146 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>463</v>
+        <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>464</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>453</v>
+        <v>356</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>463</v>
       </c>
       <c r="B133" t="s">
-        <v>357</v>
+        <v>464</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B134" t="s">
-        <v>360</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>453</v>
+        <v>357</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B135" t="s">
-        <v>359</v>
+        <v>360</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B136" t="s">
-        <v>358</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>453</v>
+        <v>359</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B137" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B138" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B139" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B140" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B141" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B142" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B143" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B144" t="s">
-        <v>368</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>453</v>
+        <v>367</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B145" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>453</v>
@@ -3242,100 +3254,100 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B146" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B147" t="s">
-        <v>371</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>453</v>
+        <v>370</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B148" t="s">
-        <v>372</v>
+        <v>371</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B149" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B150" t="s">
-        <v>374</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>453</v>
+        <v>373</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B151" t="s">
-        <v>375</v>
+        <v>374</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B152" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B153" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B154" t="s">
-        <v>378</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>453</v>
+        <v>377</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B155" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>453</v>
@@ -3346,72 +3358,78 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B156" t="s">
-        <v>380</v>
+        <v>379</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B157" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>382</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>453</v>
+        <v>381</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B159" t="s">
-        <v>383</v>
+        <v>382</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B160" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B161" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B162" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B163" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>453</v>
@@ -3422,104 +3440,104 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B164" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B165" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B166" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B167" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B168" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B169" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B170" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B171" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B172" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B173" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B174" t="s">
-        <v>398</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D174" s="3" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B175" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>453</v>
@@ -3530,10 +3548,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B176" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>453</v>
@@ -3544,56 +3562,56 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B177" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B178" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B179" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B180" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B181" t="s">
-        <v>405</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>453</v>
+        <v>404</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B182" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>453</v>
@@ -3604,72 +3622,72 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B183" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B184" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B185" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B186" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B187" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B188" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B189" t="s">
-        <v>413</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>453</v>
+        <v>412</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B190" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>453</v>
@@ -3680,130 +3698,130 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B191" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B192" t="s">
-        <v>418</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>453</v>
+        <v>415</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B193" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B194" t="s">
-        <v>417</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B195" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>461</v>
+        <v>190</v>
       </c>
       <c r="B196" t="s">
-        <v>462</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D196" s="3" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>191</v>
+        <v>461</v>
       </c>
       <c r="B197" t="s">
-        <v>420</v>
+        <v>462</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B198" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B199" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B200" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B201" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B202" t="s">
-        <v>425</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D202" s="3" t="s">
-        <v>453</v>
+        <v>424</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B203" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>453</v>
@@ -3814,156 +3832,156 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>198</v>
+        <v>470</v>
       </c>
       <c r="B204" t="s">
-        <v>427</v>
+        <v>471</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B205" t="s">
-        <v>428</v>
+        <v>426</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B206" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B207" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B208" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B209" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B210" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B211" t="s">
-        <v>434</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B212" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B213" t="s">
-        <v>436</v>
+        <v>434</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B214" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B215" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B216" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B217" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B218" t="s">
-        <v>441</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D218" s="3" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B219" t="s">
-        <v>442</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D219" s="3" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>468</v>
+        <v>212</v>
       </c>
       <c r="B220" t="s">
-        <v>469</v>
+        <v>441</v>
       </c>
       <c r="C220" s="3" t="s">
         <v>453</v>
@@ -3974,10 +3992,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B221" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>453</v>
@@ -3988,18 +4006,24 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>215</v>
+        <v>468</v>
       </c>
       <c r="B222" t="s">
-        <v>466</v>
+        <v>469</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>465</v>
+        <v>214</v>
       </c>
       <c r="B223" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>453</v>
@@ -4010,62 +4034,56 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B224" t="s">
-        <v>444</v>
+        <v>466</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>217</v>
+        <v>465</v>
       </c>
       <c r="B225" t="s">
-        <v>445</v>
+        <v>467</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B226" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B227" t="s">
-        <v>447</v>
-      </c>
-      <c r="C227" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D227" s="3" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B228" t="s">
-        <v>448</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D228" s="3" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B229" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>453</v>
@@ -4076,10 +4094,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>457</v>
+        <v>220</v>
       </c>
       <c r="B230" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>453</v>
@@ -4090,42 +4108,70 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B231" t="s">
-        <v>451</v>
+        <v>449</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>223</v>
+        <v>457</v>
       </c>
       <c r="B232" t="s">
-        <v>450</v>
+        <v>458</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>222</v>
+      </c>
+      <c r="B233" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>223</v>
+      </c>
+      <c r="B234" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
         <v>224</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B235" t="s">
         <v>452</v>
       </c>
-      <c r="C233" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C234" s="3">
-        <f>COUNTIF(C2:C233,"=Y")</f>
-        <v>74</v>
-      </c>
-      <c r="D234" s="3">
-        <f>COUNTIF(D2:D233,"=Y")</f>
-        <v>74</v>
+      <c r="C235" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C236" s="3">
+        <f>COUNTIF(C2:C235,"=Y")</f>
+        <v>77</v>
+      </c>
+      <c r="D236" s="3">
+        <f>COUNTIF(D2:D235,"=Y")</f>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add documentation for new WriteTimeSeriesToGeoJSON command.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="476">
   <si>
     <t>Add</t>
   </si>
@@ -1446,6 +1446,12 @@
   </si>
   <si>
     <t>Read time series from DELFT FEWS PI XML file.</t>
+  </si>
+  <si>
+    <t>WriteTimeSeriesToGeoJSON</t>
+  </si>
+  <si>
+    <t>Write time series to GeoJSON file.</t>
   </si>
 </sst>
 </file>
@@ -1781,13 +1787,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D236"/>
+  <dimension ref="A1:D237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D199" sqref="D199"/>
+      <selection pane="bottomRight" activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2252,6 +2258,12 @@
       <c r="B43" t="s">
         <v>267</v>
       </c>
+      <c r="C43" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -2260,6 +2272,12 @@
       <c r="B44" t="s">
         <v>268</v>
       </c>
+      <c r="C44" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -2268,6 +2286,12 @@
       <c r="B45" t="s">
         <v>269</v>
       </c>
+      <c r="C45" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -2276,6 +2300,12 @@
       <c r="B46" t="s">
         <v>271</v>
       </c>
+      <c r="C46" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -4167,10 +4197,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>457</v>
+        <v>474</v>
       </c>
       <c r="B232" t="s">
-        <v>458</v>
+        <v>475</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>453</v>
@@ -4181,42 +4211,56 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>222</v>
+        <v>457</v>
       </c>
       <c r="B233" t="s">
-        <v>451</v>
+        <v>458</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B234" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
+        <v>223</v>
+      </c>
+      <c r="B235" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>224</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>452</v>
       </c>
-      <c r="C235" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C236" s="3">
-        <f>COUNTIF(C2:C235,"=Y")</f>
-        <v>84</v>
-      </c>
-      <c r="D236" s="3">
-        <f>COUNTIF(D2:D235,"=Y")</f>
-        <v>84</v>
+      <c r="C236" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C237" s="3">
+        <f>COUNTIF(C2:C236,"=Y")+COUNTIF(C2:C236,"=NA")</f>
+        <v>92</v>
+      </c>
+      <c r="D237" s="3">
+        <f>COUNTIF(D2:D236,"=Y")+COUNTIF(D2:D236,"=NA")</f>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documenation for recent enhancements to WriteTableToGeoJSON, WriteTimeSeriesToGeoJSON, and WriteTimeSeriesToKML.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="480">
   <si>
     <t>Add</t>
   </si>
@@ -1452,6 +1452,18 @@
   </si>
   <si>
     <t>Write time series to GeoJSON file.</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Y = yes updated</t>
+  </si>
+  <si>
+    <t>NA = not applicable</t>
+  </si>
+  <si>
+    <t>Z = not needed but could be updated if necessary (e.g., numeric parameters)</t>
   </si>
 </sst>
 </file>
@@ -1787,13 +1799,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D237"/>
+  <dimension ref="A1:D240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D238" sqref="D238"/>
+      <selection pane="bottomRight" activeCell="A222" sqref="A222:XFD222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3854,6 +3866,12 @@
       <c r="B199" t="s">
         <v>421</v>
       </c>
+      <c r="C199" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
@@ -4238,6 +4256,12 @@
       <c r="B235" t="s">
         <v>450</v>
       </c>
+      <c r="C235" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
@@ -4255,12 +4279,27 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C237" s="3">
-        <f>COUNTIF(C2:C236,"=Y")+COUNTIF(C2:C236,"=NA")</f>
-        <v>92</v>
+        <f>COUNTIF(C2:C236,"=Y")+COUNTIF(C2:C236,"=NA")+COUNTIF(C2:C236,"=Z")</f>
+        <v>94</v>
       </c>
       <c r="D237" s="3">
-        <f>COUNTIF(D2:D236,"=Y")+COUNTIF(D2:D236,"=NA")</f>
-        <v>93</v>
+        <f>COUNTIF(D2:D236,"=Y")+COUNTIF(D2:D236,"=NA")+COUNTIF(D2:D236,"=Z")</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B238" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B239" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B240" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documentation for enhancements for 11.08.01 release.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="480">
   <si>
     <t>Add</t>
   </si>
@@ -1802,10 +1802,10 @@
   <dimension ref="A1:D240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C206" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A222" sqref="A222:XFD222"/>
+      <selection pane="bottomRight" activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2105,6 +2105,12 @@
       <c r="B25" t="s">
         <v>250</v>
       </c>
+      <c r="C25" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -2770,6 +2776,12 @@
       <c r="B92" t="s">
         <v>319</v>
       </c>
+      <c r="C92" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -3992,6 +4004,12 @@
       <c r="B211" t="s">
         <v>432</v>
       </c>
+      <c r="C211" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
@@ -4280,11 +4298,11 @@
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C237" s="3">
         <f>COUNTIF(C2:C236,"=Y")+COUNTIF(C2:C236,"=NA")+COUNTIF(C2:C236,"=Z")</f>
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D237" s="3">
         <f>COUNTIF(D2:D236,"=Y")+COUNTIF(D2:D236,"=NA")+COUNTIF(D2:D236,"=Z")</f>
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update NewStatisticYearTS documentation for new functionality.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="483">
   <si>
     <t>Add</t>
   </si>
@@ -1464,6 +1464,15 @@
   </si>
   <si>
     <t>Z = not needed but could be updated if necessary (e.g., numeric parameters)</t>
+  </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>SetEnsembleProperty</t>
+  </si>
+  <si>
+    <t>Set a property on the ensemble</t>
   </si>
 </sst>
 </file>
@@ -1487,12 +1496,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1507,7 +1522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1516,6 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,13 +1815,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D240"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D215" sqref="D215"/>
+      <selection pane="bottomRight" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,6 +1830,7 @@
     <col min="2" max="2" width="124.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1929,6 +1946,12 @@
       <c r="B9" t="s">
         <v>233</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -2073,6 +2096,12 @@
       <c r="B21" t="s">
         <v>244</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2141,6 +2170,12 @@
       <c r="B28" t="s">
         <v>253</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2716,6 +2751,12 @@
       <c r="B86" t="s">
         <v>313</v>
       </c>
+      <c r="C86" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
@@ -3313,7 +3354,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>139</v>
       </c>
@@ -3327,7 +3368,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>140</v>
       </c>
@@ -3341,7 +3382,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>141</v>
       </c>
@@ -3349,7 +3390,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>142</v>
       </c>
@@ -3363,7 +3404,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>143</v>
       </c>
@@ -3371,15 +3412,24 @@
         <v>372</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>144</v>
       </c>
       <c r="B150" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C150" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -3393,15 +3443,21 @@
         <v>453</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>146</v>
       </c>
       <c r="B152" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C152" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>147</v>
       </c>
@@ -3409,7 +3465,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>148</v>
       </c>
@@ -3417,7 +3473,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>149</v>
       </c>
@@ -3431,7 +3487,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>150</v>
       </c>
@@ -3445,7 +3501,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>151</v>
       </c>
@@ -3453,7 +3509,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>152</v>
       </c>
@@ -3461,7 +3517,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>153</v>
       </c>
@@ -3475,7 +3531,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>154</v>
       </c>
@@ -3493,32 +3549,32 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>481</v>
       </c>
       <c r="B162" t="s">
-        <v>385</v>
+        <v>482</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B163" t="s">
-        <v>386</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>453</v>
+        <v>385</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B164" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>453</v>
@@ -3529,110 +3585,110 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B165" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B166" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B167" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B168" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B169" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B170" t="s">
-        <v>393</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>453</v>
+        <v>392</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B171" t="s">
-        <v>395</v>
+        <v>393</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B172" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B173" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B174" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B175" t="s">
-        <v>398</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B176" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>453</v>
@@ -3643,10 +3699,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B177" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>453</v>
@@ -3657,56 +3713,56 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B178" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B179" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B180" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B181" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B182" t="s">
-        <v>405</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>453</v>
+        <v>404</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B183" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>453</v>
@@ -3717,72 +3773,72 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B184" t="s">
-        <v>407</v>
+        <v>406</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B185" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B186" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B187" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B188" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B189" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B190" t="s">
-        <v>413</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>453</v>
+        <v>412</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B191" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>453</v>
@@ -3793,76 +3849,76 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B192" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B193" t="s">
-        <v>418</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>453</v>
+        <v>415</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B194" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B195" t="s">
-        <v>417</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B196" t="s">
-        <v>419</v>
+        <v>417</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>461</v>
+        <v>190</v>
       </c>
       <c r="B197" t="s">
-        <v>462</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>191</v>
+        <v>461</v>
       </c>
       <c r="B198" t="s">
-        <v>420</v>
+        <v>462</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>453</v>
@@ -3873,13 +3929,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B199" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>453</v>
@@ -3887,34 +3943,40 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B200" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B201" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B202" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B203" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>453</v>
@@ -3925,10 +3987,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>470</v>
+        <v>196</v>
       </c>
       <c r="B204" t="s">
-        <v>471</v>
+        <v>425</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>453</v>
@@ -3939,10 +4001,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>197</v>
+        <v>470</v>
       </c>
       <c r="B205" t="s">
-        <v>426</v>
+        <v>471</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>453</v>
@@ -3953,10 +4015,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B206" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>453</v>
@@ -3967,140 +4029,140 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B207" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B208" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B209" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B210" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B211" t="s">
-        <v>432</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D211" s="3" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B212" t="s">
-        <v>433</v>
+        <v>432</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B213" t="s">
-        <v>434</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D213" s="3" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B214" t="s">
-        <v>435</v>
+        <v>434</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B215" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B216" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B217" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B218" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B219" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B220" t="s">
-        <v>441</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D220" s="3" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B221" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>453</v>
@@ -4111,10 +4173,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>468</v>
+        <v>213</v>
       </c>
       <c r="B222" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="C222" s="3" t="s">
         <v>453</v>
@@ -4125,10 +4187,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>214</v>
+        <v>468</v>
       </c>
       <c r="B223" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>453</v>
@@ -4139,62 +4201,62 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B224" t="s">
-        <v>466</v>
+        <v>443</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>465</v>
+        <v>215</v>
       </c>
       <c r="B225" t="s">
-        <v>467</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>216</v>
+        <v>465</v>
       </c>
       <c r="B226" t="s">
-        <v>444</v>
+        <v>467</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B227" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B228" t="s">
-        <v>446</v>
-      </c>
-      <c r="C228" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D228" s="3" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B229" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C229" s="3" t="s">
         <v>453</v>
@@ -4205,10 +4267,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B230" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>453</v>
@@ -4219,10 +4281,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B231" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>453</v>
@@ -4233,10 +4295,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>474</v>
+        <v>221</v>
       </c>
       <c r="B232" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>453</v>
@@ -4247,10 +4309,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>457</v>
+        <v>474</v>
       </c>
       <c r="B233" t="s">
-        <v>458</v>
+        <v>475</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>453</v>
@@ -4261,62 +4323,76 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>222</v>
+        <v>457</v>
       </c>
       <c r="B234" t="s">
-        <v>451</v>
+        <v>458</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B235" t="s">
-        <v>450</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>223</v>
+      </c>
+      <c r="B236" t="s">
+        <v>450</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
         <v>224</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B237" t="s">
         <v>452</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C237" s="3">
-        <f>COUNTIF(C2:C236,"=Y")+COUNTIF(C2:C236,"=NA")+COUNTIF(C2:C236,"=Z")</f>
-        <v>97</v>
-      </c>
-      <c r="D237" s="3">
-        <f>COUNTIF(D2:D236,"=Y")+COUNTIF(D2:D236,"=NA")+COUNTIF(D2:D236,"=Z")</f>
-        <v>98</v>
+      <c r="C237" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B238" t="s">
-        <v>477</v>
+      <c r="C238" s="3">
+        <f>COUNTIF(C2:C237,"=Y")+COUNTIF(C2:C237,"=NA")+COUNTIF(C2:C237,"=Z")</f>
+        <v>105</v>
+      </c>
+      <c r="D238" s="3">
+        <f>COUNTIF(D2:D237,"=Y")+COUNTIF(D2:D237,"=NA")+COUNTIF(D2:D237,"=Z")</f>
+        <v>106</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B239" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B240" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B241" t="s">
         <v>479</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update TSID and CreateRegressionTestCommand command documentation for updates.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="483">
   <si>
     <t>Add</t>
   </si>
@@ -1463,9 +1463,6 @@
     <t>NA = not applicable</t>
   </si>
   <si>
-    <t>Z = not needed but could be updated if necessary (e.g., numeric parameters)</t>
-  </si>
-  <si>
     <t>Deprecated</t>
   </si>
   <si>
@@ -1473,6 +1470,9 @@
   </si>
   <si>
     <t>Set a property on the ensemble</t>
+  </si>
+  <si>
+    <t>Z = not needed but could be updated if necessary (e.g., numeric parameters, more complex issues)</t>
   </si>
 </sst>
 </file>
@@ -1821,7 +1821,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C90" sqref="C90"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,6 +2247,12 @@
       <c r="B35" t="s">
         <v>259</v>
       </c>
+      <c r="C35" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -3426,7 +3432,7 @@
         <v>454</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3549,10 +3555,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>480</v>
+      </c>
+      <c r="B162" t="s">
         <v>481</v>
-      </c>
-      <c r="B162" t="s">
-        <v>482</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>453</v>
@@ -3912,6 +3918,12 @@
       <c r="B197" t="s">
         <v>419</v>
       </c>
+      <c r="C197" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
@@ -4374,11 +4386,11 @@
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C238" s="3">
         <f>COUNTIF(C2:C237,"=Y")+COUNTIF(C2:C237,"=NA")+COUNTIF(C2:C237,"=Z")</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D238" s="3">
         <f>COUNTIF(D2:D237,"=Y")+COUNTIF(D2:D237,"=NA")+COUNTIF(D2:D237,"=Z")</f>
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
@@ -4393,7 +4405,7 @@
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documentation to include HTML versions of command documentation for ReadReclamationHDB, WriteReclamationHDB, and SortTimeSeries.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="483">
   <si>
     <t>Add</t>
   </si>
@@ -1472,7 +1472,7 @@
     <t>Set a property on the ensemble</t>
   </si>
   <si>
-    <t>Z = not needed but could be updated if necessary (e.g., numeric parameters, more complex issues)</t>
+    <t>Z = not needed/updated but could be updated if necessary (e.g., numeric parameters, more complex issues)</t>
   </si>
 </sst>
 </file>
@@ -1818,10 +1818,10 @@
   <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2118,6 +2118,12 @@
       <c r="B23" t="s">
         <v>246</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2947,6 +2953,12 @@
       <c r="B103" t="s">
         <v>330</v>
       </c>
+      <c r="C103" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
@@ -3027,6 +3039,12 @@
       <c r="B110" t="s">
         <v>336</v>
       </c>
+      <c r="C110" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
@@ -3798,6 +3816,12 @@
       <c r="B185" t="s">
         <v>407</v>
       </c>
+      <c r="C185" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
@@ -4386,11 +4410,11 @@
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C238" s="3">
         <f>COUNTIF(C2:C237,"=Y")+COUNTIF(C2:C237,"=NA")+COUNTIF(C2:C237,"=Z")</f>
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D238" s="3">
         <f>COUNTIF(D2:D237,"=Y")+COUNTIF(D2:D237,"=NA")+COUNTIF(D2:D237,"=Z")</f>
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update documentation to reflect recent command enhancements.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="485">
   <si>
     <t>Add</t>
   </si>
@@ -1824,10 +1824,10 @@
   <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B164" sqref="B164"/>
+      <selection pane="bottomRight" activeCell="F194" sqref="F194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3724,6 +3724,12 @@
       <c r="B175" t="s">
         <v>396</v>
       </c>
+      <c r="C175" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
@@ -3872,6 +3878,12 @@
       <c r="B189" t="s">
         <v>410</v>
       </c>
+      <c r="C189" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
@@ -4024,6 +4036,12 @@
       <c r="B202" t="s">
         <v>422</v>
       </c>
+      <c r="C202" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
@@ -4436,11 +4454,11 @@
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C239" s="3">
         <f>COUNTIF(C2:C238,"=Y")+COUNTIF(C2:C238,"=NA")+COUNTIF(C2:C238,"=Z")</f>
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D239" s="3">
         <f>COUNTIF(D2:D238,"=Y")+COUNTIF(D2:D238,"=NA")+COUNTIF(D2:D238,"=Z")</f>
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update documentation for recent software enhancements preparing for 11.10.01 release.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="486">
   <si>
     <t>Add</t>
   </si>
@@ -1479,6 +1479,9 @@
   </si>
   <si>
     <t>Send an email message</t>
+  </si>
+  <si>
+    <t>HTML Documentation?</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1538,6 +1541,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1824,10 +1830,10 @@
   <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="E239" sqref="E239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1839,7 +1845,7 @@
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>225</v>
       </c>
@@ -1852,8 +1858,11 @@
       <c r="D1" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +1912,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1945,7 +1954,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1959,7 +1968,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1967,7 +1976,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1981,7 +1990,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2009,7 +2018,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2640,6 +2649,9 @@
       <c r="C71" s="3" t="s">
         <v>453</v>
       </c>
+      <c r="D71" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -2726,6 +2738,9 @@
       <c r="B81" t="s">
         <v>308</v>
       </c>
+      <c r="C81" s="3" t="s">
+        <v>453</v>
+      </c>
       <c r="D81" s="3" t="s">
         <v>453</v>
       </c>
@@ -3074,7 +3089,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -3082,7 +3097,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -3090,7 +3105,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -3098,7 +3113,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -3106,7 +3121,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3114,15 +3129,24 @@
         <v>343</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>115</v>
       </c>
       <c r="B118" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C118" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E118" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>459</v>
       </c>
@@ -3136,7 +3160,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -3144,7 +3168,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -3158,7 +3182,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -3166,7 +3190,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -3174,7 +3198,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -3182,7 +3206,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -3190,7 +3214,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -3198,7 +3222,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -3212,12 +3236,18 @@
         <v>453</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>124</v>
       </c>
       <c r="B128" t="s">
         <v>353</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -3745,7 +3775,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>169</v>
       </c>
@@ -3759,7 +3789,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>170</v>
       </c>
@@ -3773,7 +3803,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>171</v>
       </c>
@@ -3787,7 +3817,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -3795,7 +3825,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>173</v>
       </c>
@@ -3803,7 +3833,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>174</v>
       </c>
@@ -3811,7 +3841,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>175</v>
       </c>
@@ -3819,7 +3849,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>176</v>
       </c>
@@ -3833,7 +3863,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>177</v>
       </c>
@@ -3847,7 +3877,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>178</v>
       </c>
@@ -3860,8 +3890,11 @@
       <c r="D186" s="3" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E186" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>179</v>
       </c>
@@ -3869,7 +3902,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>180</v>
       </c>
@@ -3877,7 +3910,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>181</v>
       </c>
@@ -3891,7 +3924,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>182</v>
       </c>
@@ -3899,7 +3932,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>183</v>
       </c>
@@ -3907,7 +3940,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>184</v>
       </c>
@@ -4127,7 +4160,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>199</v>
       </c>
@@ -4135,7 +4168,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>200</v>
       </c>
@@ -4143,7 +4176,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>201</v>
       </c>
@@ -4151,7 +4184,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>202</v>
       </c>
@@ -4159,7 +4192,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>203</v>
       </c>
@@ -4172,8 +4205,11 @@
       <c r="D213" s="3" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E213" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>204</v>
       </c>
@@ -4181,7 +4217,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>205</v>
       </c>
@@ -4195,7 +4231,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>206</v>
       </c>
@@ -4203,7 +4239,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>207</v>
       </c>
@@ -4211,7 +4247,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>208</v>
       </c>
@@ -4219,7 +4255,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>209</v>
       </c>
@@ -4227,7 +4263,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>210</v>
       </c>
@@ -4235,7 +4271,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>211</v>
       </c>
@@ -4243,7 +4279,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>212</v>
       </c>
@@ -4257,7 +4293,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>213</v>
       </c>
@@ -4271,7 +4307,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>468</v>
       </c>
@@ -4285,7 +4321,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>214</v>
       </c>
@@ -4299,7 +4335,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>215</v>
       </c>
@@ -4307,7 +4343,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>465</v>
       </c>
@@ -4321,7 +4357,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>216</v>
       </c>
@@ -4329,7 +4365,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>217</v>
       </c>
@@ -4337,7 +4373,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>218</v>
       </c>
@@ -4351,7 +4387,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>219</v>
       </c>
@@ -4365,7 +4401,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>220</v>
       </c>
@@ -4379,7 +4415,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>221</v>
       </c>
@@ -4393,7 +4429,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>474</v>
       </c>
@@ -4407,7 +4443,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>457</v>
       </c>
@@ -4421,15 +4457,21 @@
         <v>453</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>222</v>
       </c>
       <c r="B236" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C236" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>223</v>
       </c>
@@ -4443,7 +4485,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>224</v>
       </c>
@@ -4457,17 +4499,21 @@
         <v>453</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C239" s="3">
         <f>COUNTIF(C2:C238,"=Y")+COUNTIF(C2:C238,"=NA")+COUNTIF(C2:C238,"=Z")</f>
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D239" s="3">
         <f>COUNTIF(D2:D238,"=Y")+COUNTIF(D2:D238,"=NA")+COUNTIF(D2:D238,"=Z")</f>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="E239" s="3">
+        <f>COUNTIF(E2:E238,"=Y")+COUNTIF(E2:E238,"=NA")+COUNTIF(E2:E238,"=Z")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B240" t="s">
         <v>477</v>
       </c>

</xml_diff>

<commit_message>
Update SplitTableRow and ManipulateTableString command documentation for recent changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="486">
   <si>
     <t>Add</t>
   </si>
@@ -1830,10 +1830,10 @@
   <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C218" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E239" sqref="E239"/>
+      <selection pane="bottomRight" activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3909,6 +3909,12 @@
       <c r="B188" t="s">
         <v>409</v>
       </c>
+      <c r="C188" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
@@ -4502,11 +4508,11 @@
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C239" s="3">
         <f>COUNTIF(C2:C238,"=Y")+COUNTIF(C2:C238,"=NA")+COUNTIF(C2:C238,"=Z")</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D239" s="3">
         <f>COUNTIF(D2:D238,"=Y")+COUNTIF(D2:D238,"=NA")+COUNTIF(D2:D238,"=Z")</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E239" s="3">
         <f>COUNTIF(E2:E238,"=Y")+COUNTIF(E2:E238,"=NA")+COUNTIF(E2:E238,"=Z")</f>

</xml_diff>

<commit_message>
Update ReadUsgsNwisRdb documentation for command changes.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="486">
   <si>
     <t>Add</t>
   </si>
@@ -1830,10 +1830,10 @@
   <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E236" sqref="E236"/>
+      <selection pane="bottomRight" activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3395,6 +3395,12 @@
       <c r="B141" t="s">
         <v>364</v>
       </c>
+      <c r="C141" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
@@ -4508,11 +4514,11 @@
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C239" s="3">
         <f>COUNTIF(C2:C238,"=Y")+COUNTIF(C2:C238,"=NA")+COUNTIF(C2:C238,"=Z")</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D239" s="3">
         <f>COUNTIF(D2:D238,"=Y")+COUNTIF(D2:D238,"=NA")+COUNTIF(D2:D238,"=Z")</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E239" s="3">
         <f>COUNTIF(E2:E238,"=Y")+COUNTIF(E2:E238,"=NA")+COUNTIF(E2:E238,"=Z")</f>

</xml_diff>

<commit_message>
Update WriteSummary documentation to include properties, add DeleteTableColumns documentation.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="488">
   <si>
     <t>Add</t>
   </si>
@@ -1482,6 +1482,12 @@
   </si>
   <si>
     <t>HTML Documentation?</t>
+  </si>
+  <si>
+    <t>DeleteTableColumns</t>
+  </si>
+  <si>
+    <t>Delete 1+ columns from a table.</t>
   </si>
 </sst>
 </file>
@@ -1827,13 +1833,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C143" sqref="C143"/>
+      <selection pane="bottomRight" activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2245,7 +2251,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2253,7 +2259,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2297,7 +2303,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2305,58 +2311,61 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>486</v>
+      </c>
+      <c r="B39" t="s">
+        <v>487</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E39" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>267</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>268</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>454</v>
@@ -2365,12 +2374,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>454</v>
@@ -2379,12 +2388,12 @@
         <v>454</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>454</v>
@@ -2393,26 +2402,26 @@
         <v>454</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>272</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>273</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>453</v>
@@ -2423,32 +2432,32 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>282</v>
+        <v>273</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>274</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>453</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>453</v>
@@ -2459,146 +2468,146 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>279</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>453</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>284</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>453</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>285</v>
+        <v>284</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>287</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>454</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>290</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>453</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>453</v>
@@ -2609,186 +2618,186 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>296</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>453</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>453</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>306</v>
+        <v>303</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>308</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>453</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>312</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>453</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>453</v>
@@ -2799,10 +2808,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>453</v>
@@ -2813,10 +2822,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>453</v>
@@ -2827,48 +2836,48 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>316</v>
+        <v>315</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>319</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>453</v>
+        <v>318</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>453</v>
@@ -2879,10 +2888,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>453</v>
@@ -2893,10 +2902,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>453</v>
@@ -2907,10 +2916,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>453</v>
@@ -2921,64 +2930,64 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>324</v>
+        <v>323</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>329</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>453</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>453</v>
@@ -2989,10 +2998,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>453</v>
@@ -3003,10 +3012,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>453</v>
@@ -3017,10 +3026,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>455</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>456</v>
+        <v>332</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>453</v>
@@ -3031,10 +3040,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>455</v>
       </c>
       <c r="B107" t="s">
-        <v>333</v>
+        <v>456</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>453</v>
@@ -3045,203 +3054,203 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>336</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>453</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
-        <v>337</v>
+        <v>336</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B113" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B114" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B115" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B116" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B117" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>344</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E118" t="s">
-        <v>453</v>
+        <v>343</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>459</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>460</v>
+        <v>344</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>453</v>
       </c>
       <c r="D119" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E119" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>459</v>
       </c>
       <c r="B120" t="s">
-        <v>345</v>
+        <v>460</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B121" t="s">
-        <v>346</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>453</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>348</v>
+        <v>346</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B124" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>352</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>453</v>
+        <v>351</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>453</v>
@@ -3252,10 +3261,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>472</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>473</v>
+        <v>353</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>453</v>
@@ -3266,10 +3275,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>472</v>
       </c>
       <c r="B130" t="s">
-        <v>354</v>
+        <v>473</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>453</v>
@@ -3280,10 +3289,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>453</v>
@@ -3294,54 +3303,54 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>463</v>
+        <v>127</v>
       </c>
       <c r="B133" t="s">
-        <v>464</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>453</v>
+        <v>356</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>128</v>
+        <v>463</v>
       </c>
       <c r="B134" t="s">
-        <v>357</v>
+        <v>464</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>360</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>453</v>
+        <v>357</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>453</v>
@@ -3352,10 +3361,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B137" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>453</v>
@@ -3366,86 +3375,86 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B138" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B141" t="s">
-        <v>364</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>453</v>
+        <v>362</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B142" t="s">
-        <v>365</v>
+        <v>364</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B143" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B144" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
-        <v>368</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>453</v>
+        <v>367</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B146" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>453</v>
@@ -3456,71 +3465,71 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>370</v>
+        <v>369</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B148" t="s">
-        <v>371</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>453</v>
+        <v>370</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B149" t="s">
-        <v>372</v>
+        <v>371</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B150" t="s">
-        <v>373</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>479</v>
+        <v>372</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B151" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B152" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>453</v>
@@ -3531,40 +3540,40 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B153" t="s">
-        <v>376</v>
+        <v>375</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B154" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B155" t="s">
-        <v>378</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>453</v>
+        <v>377</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B156" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>453</v>
@@ -3575,13 +3584,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>483</v>
+        <v>150</v>
       </c>
       <c r="B157" t="s">
-        <v>484</v>
+        <v>379</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>453</v>
@@ -3589,65 +3598,65 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>151</v>
+        <v>483</v>
       </c>
       <c r="B158" t="s">
-        <v>380</v>
+        <v>484</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B159" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B160" t="s">
-        <v>382</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>453</v>
+        <v>381</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B161" t="s">
-        <v>383</v>
+        <v>382</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B162" t="s">
-        <v>384</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>453</v>
+        <v>383</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>480</v>
+        <v>155</v>
       </c>
       <c r="B163" t="s">
-        <v>481</v>
+        <v>384</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>453</v>
@@ -3655,32 +3664,32 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>156</v>
+        <v>480</v>
       </c>
       <c r="B164" t="s">
-        <v>385</v>
+        <v>481</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B165" t="s">
-        <v>386</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>453</v>
+        <v>385</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B166" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>453</v>
@@ -3691,116 +3700,116 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B167" t="s">
-        <v>388</v>
+        <v>387</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B168" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B169" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B170" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B171" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B172" t="s">
-        <v>393</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>453</v>
+        <v>392</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B173" t="s">
-        <v>395</v>
+        <v>393</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B174" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B175" t="s">
-        <v>396</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>453</v>
+        <v>394</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B176" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B177" t="s">
-        <v>398</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B178" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>453</v>
@@ -3811,10 +3820,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B179" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>453</v>
@@ -3825,56 +3834,56 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B180" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B181" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B182" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B183" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B184" t="s">
-        <v>405</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>453</v>
+        <v>404</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B185" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>453</v>
@@ -3885,49 +3894,49 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B186" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>453</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E186" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B187" t="s">
-        <v>408</v>
+        <v>407</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E187" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B188" t="s">
-        <v>409</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B189" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>453</v>
@@ -3938,40 +3947,40 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B190" t="s">
-        <v>411</v>
+        <v>410</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B191" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B192" t="s">
-        <v>413</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>453</v>
+        <v>412</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B193" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>453</v>
@@ -3982,57 +3991,57 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B194" t="s">
-        <v>415</v>
+        <v>414</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B195" t="s">
-        <v>418</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>453</v>
+        <v>415</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B196" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B197" t="s">
-        <v>417</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B198" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>453</v>
@@ -4040,13 +4049,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>461</v>
+        <v>190</v>
       </c>
       <c r="B199" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>453</v>
@@ -4054,10 +4063,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>191</v>
+        <v>461</v>
       </c>
       <c r="B200" t="s">
-        <v>420</v>
+        <v>462</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>453</v>
@@ -4068,13 +4077,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B201" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>453</v>
@@ -4082,13 +4091,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B202" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>453</v>
@@ -4096,32 +4105,32 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B203" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B204" t="s">
-        <v>424</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>453</v>
+        <v>423</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B205" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>453</v>
@@ -4132,10 +4141,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>470</v>
+        <v>196</v>
       </c>
       <c r="B206" t="s">
-        <v>471</v>
+        <v>425</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>453</v>
@@ -4146,10 +4155,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>197</v>
+        <v>470</v>
       </c>
       <c r="B207" t="s">
-        <v>426</v>
+        <v>471</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>453</v>
@@ -4160,10 +4169,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B208" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>453</v>
@@ -4174,143 +4183,149 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B209" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B210" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B211" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B212" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B213" t="s">
-        <v>432</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D213" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E213" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B214" t="s">
-        <v>433</v>
+        <v>432</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E214" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B215" t="s">
-        <v>434</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D215" s="3" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B216" t="s">
-        <v>435</v>
+        <v>434</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B217" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B218" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B219" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B220" t="s">
-        <v>439</v>
+        <v>438</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B221" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B222" t="s">
-        <v>441</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D222" s="3" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B223" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C223" s="3" t="s">
         <v>453</v>
@@ -4321,10 +4336,10 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>468</v>
+        <v>213</v>
       </c>
       <c r="B224" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>453</v>
@@ -4335,10 +4350,10 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>214</v>
+        <v>468</v>
       </c>
       <c r="B225" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>453</v>
@@ -4349,62 +4364,62 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B226" t="s">
-        <v>466</v>
+        <v>443</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>465</v>
+        <v>215</v>
       </c>
       <c r="B227" t="s">
-        <v>467</v>
-      </c>
-      <c r="C227" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D227" s="3" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>216</v>
+        <v>465</v>
       </c>
       <c r="B228" t="s">
-        <v>444</v>
+        <v>467</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B229" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B230" t="s">
-        <v>446</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D230" s="3" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B231" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>453</v>
@@ -4415,10 +4430,10 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B232" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C232" s="3" t="s">
         <v>453</v>
@@ -4429,10 +4444,10 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B233" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>453</v>
@@ -4443,10 +4458,10 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>474</v>
+        <v>221</v>
       </c>
       <c r="B234" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>453</v>
@@ -4457,10 +4472,10 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>457</v>
+        <v>474</v>
       </c>
       <c r="B235" t="s">
-        <v>458</v>
+        <v>475</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>453</v>
@@ -4471,10 +4486,10 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>222</v>
+        <v>457</v>
       </c>
       <c r="B236" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>453</v>
@@ -4485,10 +4500,10 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B237" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>453</v>
@@ -4499,44 +4514,58 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>223</v>
+      </c>
+      <c r="B238" t="s">
+        <v>450</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
         <v>224</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>452</v>
       </c>
-      <c r="C238" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C239" s="3">
-        <f>COUNTIF(C2:C238,"=Y")+COUNTIF(C2:C238,"=NA")+COUNTIF(C2:C238,"=Z")</f>
-        <v>123</v>
-      </c>
-      <c r="D239" s="3">
-        <f>COUNTIF(D2:D238,"=Y")+COUNTIF(D2:D238,"=NA")+COUNTIF(D2:D238,"=Z")</f>
-        <v>124</v>
-      </c>
-      <c r="E239" s="3">
-        <f>COUNTIF(E2:E238,"=Y")+COUNTIF(E2:E238,"=NA")+COUNTIF(E2:E238,"=Z")</f>
-        <v>3</v>
+      <c r="C239" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B240" t="s">
-        <v>477</v>
+      <c r="C240" s="3">
+        <f>COUNTIF(C2:C239,"=Y")+COUNTIF(C2:C239,"=NA")+COUNTIF(C2:C239,"=Z")</f>
+        <v>125</v>
+      </c>
+      <c r="D240" s="3">
+        <f>COUNTIF(D2:D239,"=Y")+COUNTIF(D2:D239,"=NA")+COUNTIF(D2:D239,"=Z")</f>
+        <v>126</v>
+      </c>
+      <c r="E240" s="3">
+        <f>COUNTIF(E2:E239,"=Y")+COUNTIF(E2:E239,"=NA")+COUNTIF(E2:E239,"=Z")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B243" t="s">
         <v>482</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documentation for SelectTimeSeries and TableTimeSeriesMath commands.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="488">
   <si>
     <t>Add</t>
   </si>
@@ -1839,7 +1839,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B242" sqref="B242"/>
+      <selection pane="bottomRight" activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4010,6 +4010,12 @@
       <c r="B195" t="s">
         <v>415</v>
       </c>
+      <c r="C195" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
@@ -4543,11 +4549,11 @@
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C240" s="3">
         <f>COUNTIF(C2:C239,"=Y")+COUNTIF(C2:C239,"=NA")+COUNTIF(C2:C239,"=Z")</f>
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D240" s="3">
         <f>COUNTIF(D2:D239,"=Y")+COUNTIF(D2:D239,"=NA")+COUNTIF(D2:D239,"=Z")</f>
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E240" s="3">
         <f>COUNTIF(E2:E239,"=Y")+COUNTIF(E2:E239,"=NA")+COUNTIF(E2:E239,"=Z")</f>

</xml_diff>

<commit_message>
Update documentation for Divide, FillRepeat, and Multiply commands for properties support.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="488">
   <si>
     <t>Add</t>
   </si>
@@ -1836,10 +1836,10 @@
   <dimension ref="A1:E243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B219" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A157" sqref="A157:XFD157"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2359,6 +2359,12 @@
       <c r="B43" t="s">
         <v>266</v>
       </c>
+      <c r="C43" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -2563,6 +2569,12 @@
       <c r="B61" t="s">
         <v>285</v>
       </c>
+      <c r="C61" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -2775,6 +2787,12 @@
       <c r="B83" t="s">
         <v>309</v>
       </c>
+      <c r="C83" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -4549,11 +4567,11 @@
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C240" s="3">
         <f>COUNTIF(C2:C239,"=Y")+COUNTIF(C2:C239,"=NA")+COUNTIF(C2:C239,"=Z")</f>
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D240" s="3">
         <f>COUNTIF(D2:D239,"=Y")+COUNTIF(D2:D239,"=NA")+COUNTIF(D2:D239,"=Z")</f>
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E240" s="3">
         <f>COUNTIF(E2:E239,"=Y")+COUNTIF(E2:E239,"=NA")+COUNTIF(E2:E239,"=Z")</f>

</xml_diff>

<commit_message>
Update documentation for recent enhancements.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="488">
   <si>
     <t>Add</t>
   </si>
@@ -1836,10 +1836,10 @@
   <dimension ref="A1:E243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomRight" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3761,6 +3761,12 @@
       <c r="B171" t="s">
         <v>391</v>
       </c>
+      <c r="C171" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
@@ -4567,11 +4573,11 @@
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C240" s="3">
         <f>COUNTIF(C2:C239,"=Y")+COUNTIF(C2:C239,"=NA")+COUNTIF(C2:C239,"=Z")</f>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D240" s="3">
         <f>COUNTIF(D2:D239,"=Y")+COUNTIF(D2:D239,"=NA")+COUNTIF(D2:D239,"=Z")</f>
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E240" s="3">
         <f>COUNTIF(E2:E239,"=Y")+COUNTIF(E2:E239,"=NA")+COUNTIF(E2:E239,"=Z")</f>

</xml_diff>

<commit_message>
Update many commands to reflect support for ${Property}.  Add new chapter 11 for Model Framework Integration.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="490">
   <si>
     <t>Add</t>
   </si>
@@ -1488,6 +1488,12 @@
   </si>
   <si>
     <t>Delete 1+ columns from a table.</t>
+  </si>
+  <si>
+    <t>SetPropertyFromTimeSeries</t>
+  </si>
+  <si>
+    <t>Set a processor property from time series property.</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1549,6 +1555,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1833,13 +1842,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E243"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C219" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E171" sqref="E171"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,6 +2259,12 @@
       <c r="B32" t="s">
         <v>257</v>
       </c>
+      <c r="C32" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -2335,6 +2350,12 @@
       <c r="B40" t="s">
         <v>263</v>
       </c>
+      <c r="C40" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -2673,6 +2694,12 @@
       <c r="B71" t="s">
         <v>295</v>
       </c>
+      <c r="C71" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -2711,6 +2738,12 @@
       <c r="B75" t="s">
         <v>299</v>
       </c>
+      <c r="C75" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -3526,16 +3559,16 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="A151" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C151" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="6" t="s">
         <v>454</v>
       </c>
       <c r="E151" s="4" t="s">
@@ -3577,6 +3610,12 @@
       <c r="B154" t="s">
         <v>376</v>
       </c>
+      <c r="C154" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
@@ -3805,13 +3844,19 @@
       <c r="B175" t="s">
         <v>394</v>
       </c>
+      <c r="C175" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>167</v>
+        <v>488</v>
       </c>
       <c r="B176" t="s">
-        <v>396</v>
+        <v>489</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>453</v>
@@ -3822,32 +3867,32 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B177" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B178" t="s">
-        <v>398</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B179" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>453</v>
@@ -3858,10 +3903,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B180" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>453</v>
@@ -3872,42 +3917,48 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B181" t="s">
-        <v>402</v>
+        <v>399</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B182" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B183" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B184" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B185" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>453</v>
@@ -3918,10 +3969,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B186" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>453</v>
@@ -3932,49 +3983,49 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B187" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>453</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E187" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B188" t="s">
-        <v>408</v>
+        <v>407</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E188" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B189" t="s">
-        <v>409</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D189" s="3" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B190" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>453</v>
@@ -3985,40 +4036,40 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B191" t="s">
-        <v>411</v>
+        <v>410</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B192" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B193" t="s">
-        <v>413</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>453</v>
+        <v>412</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B194" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>453</v>
@@ -4029,10 +4080,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B195" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>453</v>
@@ -4043,10 +4094,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B196" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>453</v>
@@ -4057,35 +4108,35 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B197" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B198" t="s">
-        <v>417</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D198" s="3" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B199" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>453</v>
@@ -4093,13 +4144,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>461</v>
+        <v>190</v>
       </c>
       <c r="B200" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>453</v>
@@ -4107,10 +4158,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>191</v>
+        <v>461</v>
       </c>
       <c r="B201" t="s">
-        <v>420</v>
+        <v>462</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>453</v>
@@ -4121,13 +4172,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B202" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>453</v>
@@ -4135,13 +4186,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B203" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>453</v>
@@ -4149,32 +4200,32 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B204" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B205" t="s">
-        <v>424</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D205" s="3" t="s">
-        <v>453</v>
+        <v>423</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B206" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>453</v>
@@ -4185,10 +4236,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>470</v>
+        <v>196</v>
       </c>
       <c r="B207" t="s">
-        <v>471</v>
+        <v>425</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>453</v>
@@ -4199,10 +4250,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>197</v>
+        <v>470</v>
       </c>
       <c r="B208" t="s">
-        <v>426</v>
+        <v>471</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>453</v>
@@ -4213,10 +4264,10 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B209" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C209" s="3" t="s">
         <v>453</v>
@@ -4227,375 +4278,401 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B210" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B211" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B212" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B213" t="s">
-        <v>431</v>
+        <v>430</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B214" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>453</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E214" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B215" t="s">
-        <v>433</v>
+        <v>432</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E215" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B216" t="s">
-        <v>434</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B217" t="s">
-        <v>435</v>
+        <v>434</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B218" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B219" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B220" t="s">
-        <v>438</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D220" s="3" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B221" t="s">
-        <v>439</v>
+        <v>438</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B222" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B223" t="s">
-        <v>441</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D223" s="3" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>212</v>
+      </c>
+      <c r="B224" t="s">
+        <v>441</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
         <v>213</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B225" t="s">
         <v>442</v>
       </c>
-      <c r="C224" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D224" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A225" t="s">
+      <c r="C225" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
         <v>468</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B226" t="s">
         <v>469</v>
       </c>
-      <c r="C225" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A226" t="s">
+      <c r="C226" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
         <v>214</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B227" t="s">
         <v>443</v>
       </c>
-      <c r="C226" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D226" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A227" t="s">
+      <c r="C227" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
         <v>215</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B228" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
         <v>465</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B229" t="s">
         <v>467</v>
       </c>
-      <c r="C228" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D228" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229" t="s">
+      <c r="C229" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
         <v>216</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B230" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
         <v>217</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
         <v>218</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>446</v>
       </c>
-      <c r="C231" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D231" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
+      <c r="C232" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>219</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>447</v>
       </c>
-      <c r="C232" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
+      <c r="C233" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>220</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>448</v>
       </c>
-      <c r="C233" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
+      <c r="C234" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
         <v>221</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>449</v>
       </c>
-      <c r="C234" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D234" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
+      <c r="C235" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>474</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>475</v>
       </c>
-      <c r="C235" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
+      <c r="C236" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
         <v>457</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B237" t="s">
         <v>458</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A237" t="s">
+      <c r="C237" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
         <v>222</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B238" t="s">
         <v>451</v>
       </c>
-      <c r="C237" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+      <c r="C238" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
         <v>223</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>450</v>
       </c>
-      <c r="C238" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D238" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
+      <c r="C239" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
         <v>224</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B240" t="s">
         <v>452</v>
       </c>
-      <c r="C239" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D239" s="3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C240" s="3">
-        <f>COUNTIF(C2:C239,"=Y")+COUNTIF(C2:C239,"=NA")+COUNTIF(C2:C239,"=Z")</f>
-        <v>130</v>
-      </c>
-      <c r="D240" s="3">
-        <f>COUNTIF(D2:D239,"=Y")+COUNTIF(D2:D239,"=NA")+COUNTIF(D2:D239,"=Z")</f>
-        <v>131</v>
-      </c>
-      <c r="E240" s="3">
-        <f>COUNTIF(E2:E239,"=Y")+COUNTIF(E2:E239,"=NA")+COUNTIF(E2:E239,"=Z")</f>
+      <c r="C240" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C241" s="3">
+        <f>COUNTIF(C2:C240,"=Y")+COUNTIF(C2:C240,"=NA")+COUNTIF(C2:C240,"=Z")</f>
+        <v>140</v>
+      </c>
+      <c r="D241" s="3">
+        <f>COUNTIF(D2:D240,"=Y")+COUNTIF(D2:D240,"=NA")+COUNTIF(D2:D240,"=Z")</f>
+        <v>141</v>
+      </c>
+      <c r="E241" s="3">
+        <f>COUNTIF(E2:E240,"=Y")+COUNTIF(E2:E240,"=NA")+COUNTIF(E2:E240,"=Z")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B241" t="s">
+    <row r="242" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B242" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B242" t="s">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B243" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B243" t="s">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B244" t="s">
         <v>482</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update documentation for recent USGS NWIS command changes
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="490">
   <si>
     <t>Add</t>
   </si>
@@ -1848,7 +1848,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3445,6 +3445,12 @@
       <c r="B139" t="s">
         <v>361</v>
       </c>
+      <c r="C139" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
@@ -3461,6 +3467,12 @@
       <c r="B141" t="s">
         <v>362</v>
       </c>
+      <c r="C141" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
@@ -4650,11 +4662,11 @@
     <row r="241" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C241" s="3">
         <f>COUNTIF(C2:C240,"=Y")+COUNTIF(C2:C240,"=NA")+COUNTIF(C2:C240,"=Z")</f>
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D241" s="3">
         <f>COUNTIF(D2:D240,"=Y")+COUNTIF(D2:D240,"=NA")+COUNTIF(D2:D240,"=Z")</f>
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E241" s="3">
         <f>COUNTIF(E2:E240,"=Y")+COUNTIF(E2:E240,"=NA")+COUNTIF(E2:E240,"=Z")</f>

</xml_diff>

<commit_message>
Add SetPropertyFromEnsemble command.  Many other changes based on implementation of SNODAS products.
</commit_message>
<xml_diff>
--- a/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
+++ b/doc/DeveloperResources/CommandInventory/TSTool-Command-List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\owf-gitrepos\cdss-app-tstool-doc\doc\DeveloperResources\CommandInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam\cdss-dev\TSTool\git-repos\cdss-app-tstool-doc\doc\DeveloperResources\CommandInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="492">
   <si>
     <t>Add</t>
   </si>
@@ -1494,6 +1494,12 @@
   </si>
   <si>
     <t>Set a processor property from time series property.</t>
+  </si>
+  <si>
+    <t>Remaining to do</t>
+  </si>
+  <si>
+    <t>Total commands updated</t>
   </si>
 </sst>
 </file>
@@ -1842,13 +1848,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B162" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E139" sqref="E139"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,6 +2279,12 @@
       <c r="B33" t="s">
         <v>258</v>
       </c>
+      <c r="C33" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -2634,6 +2646,12 @@
       <c r="B65" t="s">
         <v>288</v>
       </c>
+      <c r="C65" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -2670,6 +2688,12 @@
       <c r="B68" t="s">
         <v>292</v>
       </c>
+      <c r="C68" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -2678,6 +2702,12 @@
       <c r="B69" t="s">
         <v>293</v>
       </c>
+      <c r="C69" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -3194,6 +3224,12 @@
       <c r="B117" t="s">
         <v>342</v>
       </c>
+      <c r="C117" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
@@ -4659,32 +4695,46 @@
         <v>453</v>
       </c>
     </row>
-    <row r="241" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C241" s="3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>491</v>
+      </c>
+      <c r="C242" s="3">
         <f>COUNTIF(C2:C240,"=Y")+COUNTIF(C2:C240,"=NA")+COUNTIF(C2:C240,"=Z")</f>
-        <v>142</v>
-      </c>
-      <c r="D241" s="3">
+        <v>147</v>
+      </c>
+      <c r="D242" s="3">
         <f>COUNTIF(D2:D240,"=Y")+COUNTIF(D2:D240,"=NA")+COUNTIF(D2:D240,"=Z")</f>
-        <v>143</v>
-      </c>
-      <c r="E241" s="3">
+        <v>148</v>
+      </c>
+      <c r="E242" s="3">
         <f>COUNTIF(E2:E240,"=Y")+COUNTIF(E2:E240,"=NA")+COUNTIF(E2:E240,"=Z")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B242" t="s">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>490</v>
+      </c>
+      <c r="B243" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B243" t="s">
+      <c r="C243" s="3">
+        <f>ROW() - 3 - C242</f>
+        <v>93</v>
+      </c>
+      <c r="D243" s="3">
+        <f>ROW() - 3 - D242</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B244" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B244" t="s">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B245" t="s">
         <v>482</v>
       </c>
     </row>

</xml_diff>